<commit_message>
Added directory for power supply board and sch too!
also added app notes for sizing power transformers!!!!!
</commit_message>
<xml_diff>
--- a/Measurements/All Filters.xlsx
+++ b/Measurements/All Filters.xlsx
@@ -95,8 +95,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -106,11 +108,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1062,7 +1066,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0295937312551771"/>
+          <c:y val="0.0336134453781513"/>
+          <c:w val="0.847172780851003"/>
+          <c:h val="0.956302521008403"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -1903,16 +1917,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>89</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>129</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2256,10 +2270,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D123"/>
+  <dimension ref="A1:D128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="D87" activeCellId="3" sqref="A4:A41 D4:D41 D45:D82 D87:D123"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3844,6 +3858,18 @@
       <c r="D123" s="1">
         <f t="shared" si="2"/>
         <v>-20</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="B128" s="1">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="C128" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="D128" s="1">
+        <f t="shared" ref="D128" si="3">20*LOG(C128/B128)</f>
+        <v>29.808217143006988</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added plans for power supply case
</commit_message>
<xml_diff>
--- a/Measurements/All Filters.xlsx
+++ b/Measurements/All Filters.xlsx
@@ -353,11 +353,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2130712280"/>
-        <c:axId val="2130715240"/>
+        <c:axId val="2134456664"/>
+        <c:axId val="2121506792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2130712280"/>
+        <c:axId val="2134456664"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -369,12 +369,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130715240"/>
+        <c:crossAx val="2121506792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2130715240"/>
+        <c:axId val="2121506792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -385,14 +385,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130712280"/>
+        <c:crossAx val="2134456664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -662,11 +661,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2132242632"/>
-        <c:axId val="2132517464"/>
+        <c:axId val="2120590424"/>
+        <c:axId val="2120605896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2132242632"/>
+        <c:axId val="2120590424"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -678,12 +677,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132517464"/>
+        <c:crossAx val="2120605896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2132517464"/>
+        <c:axId val="2120605896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -694,14 +693,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132242632"/>
+        <c:crossAx val="2120590424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -995,11 +993,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2132571048"/>
-        <c:axId val="2132229352"/>
+        <c:axId val="2120468840"/>
+        <c:axId val="2132147160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2132571048"/>
+        <c:axId val="2120468840"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1012,12 +1010,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132229352"/>
+        <c:crossAx val="2132147160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2132229352"/>
+        <c:axId val="2132147160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1028,7 +1026,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132571048"/>
+        <c:crossAx val="2120468840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1769,11 +1767,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2134473016"/>
-        <c:axId val="2134606520"/>
+        <c:axId val="2132176760"/>
+        <c:axId val="2135355368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2134473016"/>
+        <c:axId val="2132176760"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1785,12 +1783,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134606520"/>
+        <c:crossAx val="2135355368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2134606520"/>
+        <c:axId val="2135355368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1801,7 +1799,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134473016"/>
+        <c:crossAx val="2132176760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2272,7 +2270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
       <selection activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
@@ -2323,7 +2321,7 @@
         <v>0.21</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D41" si="0">20*LOG(C5/B5)</f>
+        <f t="shared" ref="D5:D24" si="0">20*LOG(C5/B5)</f>
         <v>-1.159838939553735</v>
       </c>
     </row>
@@ -2850,7 +2848,7 @@
         <v>0.8</v>
       </c>
       <c r="D54">
-        <f t="shared" ref="D46:D82" si="1">20*LOG(C54/B54)</f>
+        <f t="shared" ref="D54:D82" si="1">20*LOG(C54/B54)</f>
         <v>-49.172756980512986</v>
       </c>
     </row>
@@ -3874,7 +3872,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>